<commit_message>
Added link to immunogenetics article
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rick/Documents/GitHub/shiny_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDBE15C-8966-C946-9CF4-0C3D70ACFAC6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435440B4-8F6E-E240-824B-BD9FAD8A6438}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="600" windowWidth="32260" windowHeight="17440" xr2:uid="{70BA3954-2C7E-6E4C-97ED-000ADC449751}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="161">
   <si>
     <t>Type</t>
   </si>
@@ -504,7 +504,10 @@
     <t>Wills, S, Beaufreres, H, Brisson, B, Fraser, RS, Smith, DA</t>
   </si>
   <si>
-    <t>Accepted</t>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007%2Fs00251-018-1061-7</t>
   </si>
 </sst>
 </file>
@@ -885,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D461B22-909B-FF45-B177-E50FA7BA2062}">
   <dimension ref="B1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2234,7 +2237,7 @@
         <v>17</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
VII article in press.
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="161">
   <si>
     <t>Type</t>
   </si>
@@ -128,7 +128,7 @@
     <t>conference</t>
   </si>
   <si>
-    <t>Fraser, RS, Snyman, HN, Hammermueller, JD, Meyer, A, Lumsden, JS, Arroyo LH, Hayes, MA, Lillie BN. </t>
+    <t>Fraser, RS, Snyman, HN, Hammermueller, JD, Meyer, A, Lumsden, JS, Arroyo LH, Hayes, MA, Lillie BN.</t>
   </si>
   <si>
     <t>2016-12-03</t>
@@ -260,7 +260,7 @@
     <t>2015-11-18</t>
   </si>
   <si>
-    <t>Investigating infectious disease susceptibility in horses through targeted next-generation resequencing of the collagenous lectin gene family. </t>
+    <t>Investigating infectious disease susceptibility in horses through targeted next-generation resequencing of the collagenous lectin gene family.</t>
   </si>
   <si>
     <t>Fraser, RS, Meyer, A, Hammermueller, JD, Lillie, BN</t>
@@ -456,9 +456,6 @@
   </si>
   <si>
     <t>Veterinary Immunology and Immunopathology</t>
-  </si>
-  <si>
-    <t>Under review</t>
   </si>
   <si>
     <t>Snyman, HN, Fraser, RS, Meyer, A, Hammermueller, JD, Squires, EJ, Caswell, JL, Hayes, MA, Lillie, BN</t>
@@ -608,7 +605,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,43 +703,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:R27"/>
+  <dimension ref="B2:R27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.662962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="69.4962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="8" style="1" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.1666666666667"/>
-    <col collapsed="false" hidden="false" max="17" min="13" style="1" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.662962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="69.4962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.1666666666667"/>
+    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="10.8333333333333"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
-      <c r="P1" s="0"/>
-      <c r="Q1" s="0"/>
-    </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -921,11 +900,9 @@
       <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="0"/>
       <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="0"/>
       <c r="K5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1875,7 +1852,7 @@
         <v>146</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>19</v>
@@ -1910,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>139</v>
@@ -1922,10 +1899,10 @@
         <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>19</v>
@@ -1963,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>139</v>
@@ -1975,10 +1952,10 @@
         <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>19</v>
@@ -2016,7 +1993,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>139</v>
@@ -2028,40 +2005,40 @@
         <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,7 +2046,7 @@
         <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>103</v>
@@ -2081,13 +2058,13 @@
         <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="R27" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added link to VI&I paper
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russellfraser/Documents/GitHub/shiny_cv/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8014D5F-FEE3-1C4D-9290-1EB46A55E7B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="370" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27280" windowHeight="16560" tabRatio="370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="162">
   <si>
     <t>Type</t>
   </si>
@@ -498,17 +503,16 @@
   </si>
   <si>
     <t>https://blog.wellcome.ac.uk/2012/11/29/the-strange-future-of-antibiotics/</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0165242717305536</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -517,22 +521,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -547,7 +536,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -564,7 +553,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -572,69 +561,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -693,36 +639,344 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.662962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="69.4962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.1666666666667"/>
-    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5296296296296"/>
+    <col min="1" max="1" width="10.5"/>
+    <col min="2" max="2" width="14"/>
+    <col min="3" max="3" width="61.6640625"/>
+    <col min="4" max="6" width="10.83203125"/>
+    <col min="7" max="7" width="69.5"/>
+    <col min="8" max="11" width="10.83203125"/>
+    <col min="12" max="12" width="24.1640625"/>
+    <col min="13" max="17" width="10.83203125"/>
+    <col min="18" max="1025" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +1029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -824,11 +1078,11 @@
       <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -877,11 +1131,11 @@
       <c r="Q4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
@@ -928,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -981,7 +1235,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1034,7 +1288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1087,7 +1341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1140,7 +1394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1193,7 +1447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1246,7 +1500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1352,7 +1606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1405,7 +1659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1458,7 +1712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1511,7 +1765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1564,7 +1818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1617,7 +1871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1670,7 +1924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1723,14 +1977,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>2017</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -1776,7 +2030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:18" ht="80" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1829,7 +2083,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
@@ -1879,10 +2133,10 @@
         <v>19</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1935,7 +2189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1988,7 +2242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2295,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2069,15 +2323,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R22" r:id="rId1" display="https://doi.org/10.30802/AALAS-CM-17-000109"/>
-    <hyperlink ref="R27" r:id="rId2" display="https://blog.wellcome.ac.uk/2012/11/29/the-strange-future-of-antibiotics/"/>
+    <hyperlink ref="R22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="R27" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the Comp Med link
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russellfraser/Documents/GitHub/shiny_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8014D5F-FEE3-1C4D-9290-1EB46A55E7B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4353FD8-2C72-6644-8A8D-9C5CC1C6943D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="27280" windowHeight="16560" tabRatio="370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="164">
   <si>
     <t>Type</t>
   </si>
@@ -451,9 +451,6 @@
     <t>In press</t>
   </si>
   <si>
-    <t>https://doi.org/10.30802/AALAS-CM-17-000109</t>
-  </si>
-  <si>
     <t>Fraser, RS, Arroyo, LG, Meyer, A, Lillie, BN</t>
   </si>
   <si>
@@ -506,6 +503,15 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S0165242717305536</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>208-211</t>
+  </si>
+  <si>
+    <t>http://www.ingentaconnect.com/content/aalas/cm/2018/00000068/00000003/art00003</t>
   </si>
 </sst>
 </file>
@@ -959,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2030,7 +2036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2053,10 +2059,10 @@
         <v>141</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>19</v>
@@ -2080,7 +2086,7 @@
         <v>19</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
@@ -2088,7 +2094,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>139</v>
@@ -2100,10 +2106,10 @@
         <v>19</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>142</v>
@@ -2133,7 +2139,7 @@
         <v>19</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
@@ -2141,7 +2147,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>139</v>
@@ -2153,10 +2159,10 @@
         <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>19</v>
@@ -2194,7 +2200,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>139</v>
@@ -2206,10 +2212,10 @@
         <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>19</v>
@@ -2247,7 +2253,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>139</v>
@@ -2259,40 +2265,40 @@
         <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
@@ -2300,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>103</v>
@@ -2312,19 +2318,18 @@
         <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="R27" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="R27" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="R27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Updated bib info for VII
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rick/Documents/GitHub/shiny_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA4FADF-4B24-C04B-81DE-FE4D50411C67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DE5A70-5495-7248-90A0-D55EBF377919}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27280" windowHeight="16560" tabRatio="370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="166">
   <si>
     <t>Type</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Comparitive Medicine</t>
   </si>
   <si>
-    <t>In press</t>
-  </si>
-  <si>
     <t>Fraser, RS, Arroyo, LG, Meyer, A, Lillie, BN</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>https://blog.wellcome.ac.uk/2012/11/29/the-strange-future-of-antibiotics/</t>
   </si>
   <si>
-    <t>https://www.sciencedirect.com/science/article/pii/S0165242717305536</t>
-  </si>
-  <si>
     <t>68</t>
   </si>
   <si>
@@ -515,6 +509,15 @@
   </si>
   <si>
     <t>533-546</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>153-63</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0165242717305536?via%3Dihub</t>
   </si>
 </sst>
 </file>
@@ -969,7 +972,7 @@
   <dimension ref="B2:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,34 +2065,34 @@
         <v>141</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
@@ -2097,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>139</v>
@@ -2109,16 +2112,16 @@
         <v>19</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>19</v>
@@ -2142,7 +2145,7 @@
         <v>19</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
@@ -2150,7 +2153,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>139</v>
@@ -2162,10 +2165,10 @@
         <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>19</v>
@@ -2203,7 +2206,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>139</v>
@@ -2215,10 +2218,10 @@
         <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>19</v>
@@ -2256,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>139</v>
@@ -2268,40 +2271,40 @@
         <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
@@ -2309,7 +2312,7 @@
         <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>103</v>
@@ -2321,13 +2324,13 @@
         <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="R27" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>